<commit_message>
Add .py file + example to keep the formatting
</commit_message>
<xml_diff>
--- a/Example/Output/Canada.xlsx
+++ b/Example/Output/Canada.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bananatree\Desktop\CurrentRegion_UsedRange\Example\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bananatree\Desktop\split-excel-sheet-into-workbook-only-values\Example\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{044343AE-6A9F-4767-B5FF-1245759E237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EE45FDC-1CE6-43B4-B75D-05EBB2644DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{A898B689-2C93-4208-B48F-82675FA26594}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{2B103448-3600-478C-9893-AE8DF06ACD63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Canada" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,16 +168,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF005691"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,12 +205,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,57 +543,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3836B53B-7F8A-4229-9E1C-91C1E627B328}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F220B05A-4D10-4096-B68B-02896C247CC4}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -580,7 +641,7 @@
       <c r="G2">
         <v>20</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>32370</v>
       </c>
       <c r="I2">
@@ -627,7 +688,7 @@
       <c r="G3">
         <v>12</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>30216</v>
       </c>
       <c r="I3">
@@ -674,7 +735,7 @@
       <c r="G4">
         <v>125</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>333187.5</v>
       </c>
       <c r="I4">
@@ -721,7 +782,7 @@
       <c r="G5">
         <v>125</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>43125</v>
       </c>
       <c r="I5">
@@ -768,7 +829,7 @@
       <c r="G6">
         <v>20</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>5840</v>
       </c>
       <c r="I6">
@@ -815,7 +876,7 @@
       <c r="G7">
         <v>12</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>30216</v>
       </c>
       <c r="I7">
@@ -862,7 +923,7 @@
       <c r="G8">
         <v>350</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>603750</v>
       </c>
       <c r="I8">
@@ -909,7 +970,7 @@
       <c r="G9">
         <v>15</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>32280</v>
       </c>
       <c r="I9">
@@ -956,7 +1017,7 @@
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>36340</v>
       </c>
       <c r="I10">
@@ -1003,7 +1064,7 @@
       <c r="G11">
         <v>125</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>43125</v>
       </c>
       <c r="I11">
@@ -1050,7 +1111,7 @@
       <c r="G12">
         <v>300</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>600300</v>
       </c>
       <c r="I12">
@@ -1097,7 +1158,7 @@
       <c r="G13">
         <v>20</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>36340</v>
       </c>
       <c r="I13">
@@ -1144,7 +1205,7 @@
       <c r="G14">
         <v>7</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>9282</v>
       </c>
       <c r="I14">
@@ -1191,7 +1252,7 @@
       <c r="G15">
         <v>12</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>17340</v>
       </c>
       <c r="I15">
@@ -1238,7 +1299,7 @@
       <c r="G16">
         <v>7</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>12810</v>
       </c>
       <c r="I16">
@@ -1285,7 +1346,7 @@
       <c r="G17">
         <v>125</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <v>115375</v>
       </c>
       <c r="I17">
@@ -1332,7 +1393,7 @@
       <c r="G18">
         <v>7</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>14644</v>
       </c>
       <c r="I18">
@@ -1379,7 +1440,7 @@
       <c r="G19">
         <v>350</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>330225</v>
       </c>
       <c r="I19">
@@ -1426,7 +1487,7 @@
       <c r="G20">
         <v>125</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>92812.5</v>
       </c>
       <c r="I20">
@@ -1473,7 +1534,7 @@
       <c r="G21">
         <v>12</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <v>15540</v>
       </c>
       <c r="I21">
@@ -1520,7 +1581,7 @@
       <c r="G22">
         <v>350</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>998200</v>
       </c>
       <c r="I22">
@@ -1567,7 +1628,7 @@
       <c r="G23">
         <v>15</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <v>35445</v>
       </c>
       <c r="I23">
@@ -1614,7 +1675,7 @@
       <c r="G24">
         <v>12</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <v>15540</v>
       </c>
       <c r="I24">
@@ -1661,7 +1722,7 @@
       <c r="G25">
         <v>300</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>574800</v>
       </c>
       <c r="I25">
@@ -1708,7 +1769,7 @@
       <c r="G26">
         <v>350</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>998200</v>
       </c>
       <c r="I26">
@@ -1755,7 +1816,7 @@
       <c r="G27">
         <v>125</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="2">
         <v>341125</v>
       </c>
       <c r="I27">
@@ -1802,7 +1863,7 @@
       <c r="G28">
         <v>125</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <v>341125</v>
       </c>
       <c r="I28">
@@ -1849,7 +1910,7 @@
       <c r="G29">
         <v>300</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="2">
         <v>574800</v>
       </c>
       <c r="I29">
@@ -1896,7 +1957,7 @@
       <c r="G30">
         <v>12</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>10896</v>
       </c>
       <c r="I30">
@@ -1943,7 +2004,7 @@
       <c r="G31">
         <v>125</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>221750</v>
       </c>
       <c r="I31">
@@ -1990,7 +2051,7 @@
       <c r="G32">
         <v>125</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>251125</v>
       </c>
       <c r="I32">
@@ -2037,7 +2098,7 @@
       <c r="G33">
         <v>125</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>251125</v>
       </c>
       <c r="I33">
@@ -2084,7 +2145,7 @@
       <c r="G34">
         <v>300</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <v>562200</v>
       </c>
       <c r="I34">
@@ -2131,7 +2192,7 @@
       <c r="G35">
         <v>20</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="2">
         <v>16620</v>
       </c>
       <c r="I35">
@@ -2178,7 +2239,7 @@
       <c r="G36">
         <v>20</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <v>77010</v>
       </c>
       <c r="I36">
@@ -2225,7 +2286,7 @@
       <c r="G37">
         <v>7</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="2">
         <v>19957</v>
       </c>
       <c r="I37">
@@ -2272,7 +2333,7 @@
       <c r="G38">
         <v>15</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <v>29505</v>
       </c>
       <c r="I38">
@@ -2319,7 +2380,7 @@
       <c r="G39">
         <v>7</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="2">
         <v>19957</v>
       </c>
       <c r="I39">
@@ -2366,7 +2427,7 @@
       <c r="G40">
         <v>7</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <v>29757</v>
       </c>
       <c r="I40">
@@ -2413,7 +2474,7 @@
       <c r="G41">
         <v>15</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>3270</v>
       </c>
       <c r="I41">
@@ -2460,7 +2521,7 @@
       <c r="G42">
         <v>20</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>41480</v>
       </c>
       <c r="I42">
@@ -2507,7 +2568,7 @@
       <c r="G43">
         <v>20</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>52920</v>
       </c>
       <c r="I43">
@@ -2554,7 +2615,7 @@
       <c r="G44">
         <v>350</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>622300</v>
       </c>
       <c r="I44">
@@ -2601,7 +2662,7 @@
       <c r="G45">
         <v>7</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>16443</v>
       </c>
       <c r="I45">
@@ -2648,7 +2709,7 @@
       <c r="G46">
         <v>12</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="2">
         <v>29172</v>
       </c>
       <c r="I46">
@@ -2695,7 +2756,7 @@
       <c r="G47">
         <v>12</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="2">
         <v>29172</v>
       </c>
       <c r="I47">
@@ -2742,7 +2803,7 @@
       <c r="G48">
         <v>350</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="2">
         <v>429800</v>
       </c>
       <c r="I48">
@@ -2789,7 +2850,7 @@
       <c r="G49">
         <v>20</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2">
         <v>27780</v>
       </c>
       <c r="I49">
@@ -2836,7 +2897,7 @@
       <c r="G50">
         <v>20</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>36040</v>
       </c>
       <c r="I50">
@@ -2883,7 +2944,7 @@
       <c r="G51">
         <v>20</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <v>27780</v>
       </c>
       <c r="I51">
@@ -2930,7 +2991,7 @@
       <c r="G52">
         <v>350</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <v>193200</v>
       </c>
       <c r="I52">
@@ -2977,7 +3038,7 @@
       <c r="G53">
         <v>350</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="2">
         <v>429800</v>
       </c>
       <c r="I53">
@@ -3024,7 +3085,7 @@
       <c r="G54">
         <v>15</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="2">
         <v>42660</v>
       </c>
       <c r="I54">
@@ -3071,7 +3132,7 @@
       <c r="G55">
         <v>12</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>27588</v>
       </c>
       <c r="I55">
@@ -3118,7 +3179,7 @@
       <c r="G56">
         <v>12</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="2">
         <v>27588</v>
       </c>
       <c r="I56">
@@ -3165,7 +3226,7 @@
       <c r="G57">
         <v>125</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="2">
         <v>119000</v>
       </c>
       <c r="I57">
@@ -3212,7 +3273,7 @@
       <c r="G58">
         <v>15</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="2">
         <v>42660</v>
       </c>
       <c r="I58">
@@ -3259,7 +3320,7 @@
       <c r="G59">
         <v>300</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="2">
         <v>730800</v>
       </c>
       <c r="I59">
@@ -3306,7 +3367,7 @@
       <c r="G60">
         <v>12</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="2">
         <v>22608</v>
       </c>
       <c r="I60">
@@ -3353,7 +3414,7 @@
       <c r="G61">
         <v>15</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="2">
         <v>18930</v>
       </c>
       <c r="I61">
@@ -3400,7 +3461,7 @@
       <c r="G62">
         <v>7</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="2">
         <v>7945</v>
       </c>
       <c r="I62">
@@ -3447,7 +3508,7 @@
       <c r="G63">
         <v>7</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="2">
         <v>11074</v>
       </c>
       <c r="I63">
@@ -3494,7 +3555,7 @@
       <c r="G64">
         <v>7</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="2">
         <v>11074</v>
       </c>
       <c r="I64">
@@ -3541,7 +3602,7 @@
       <c r="G65">
         <v>7</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="2">
         <v>7945</v>
       </c>
       <c r="I65">
@@ -3588,7 +3649,7 @@
       <c r="G66">
         <v>300</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="2">
         <v>510600</v>
       </c>
       <c r="I66">
@@ -3635,7 +3696,7 @@
       <c r="G67">
         <v>300</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="2">
         <v>421200</v>
       </c>
       <c r="I67">
@@ -3682,7 +3743,7 @@
       <c r="G68">
         <v>12</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="2">
         <v>38934</v>
       </c>
       <c r="I68">
@@ -3729,7 +3790,7 @@
       <c r="G69">
         <v>125</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="2">
         <v>205625</v>
       </c>
       <c r="I69">
@@ -3776,7 +3837,7 @@
       <c r="G70">
         <v>20</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="2">
         <v>22360</v>
       </c>
       <c r="I70">
@@ -3823,7 +3884,7 @@
       <c r="G71">
         <v>7</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="2">
         <v>3416</v>
       </c>
       <c r="I71">
@@ -3870,7 +3931,7 @@
       <c r="G72">
         <v>7</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="2">
         <v>1799</v>
       </c>
       <c r="I72">
@@ -3917,7 +3978,7 @@
       <c r="G73">
         <v>20</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="2">
         <v>14160</v>
       </c>
       <c r="I73">
@@ -3964,7 +4025,7 @@
       <c r="G74">
         <v>300</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="2">
         <v>384900</v>
       </c>
       <c r="I74">
@@ -4011,7 +4072,7 @@
       <c r="G75">
         <v>12</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="2">
         <v>7176</v>
       </c>
       <c r="I75">
@@ -4058,7 +4119,7 @@
       <c r="G76">
         <v>300</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="2">
         <v>640200</v>
       </c>
       <c r="I76">
@@ -4105,7 +4166,7 @@
       <c r="G77">
         <v>20</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="2">
         <v>14160</v>
       </c>
       <c r="I77">
@@ -4152,7 +4213,7 @@
       <c r="G78">
         <v>300</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="2">
         <v>328200</v>
       </c>
       <c r="I78">
@@ -4199,7 +4260,7 @@
       <c r="G79">
         <v>300</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="2">
         <v>1140750</v>
       </c>
       <c r="I79">
@@ -4246,7 +4307,7 @@
       <c r="G80">
         <v>12</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="2">
         <v>27852</v>
       </c>
       <c r="I80">
@@ -4293,7 +4354,7 @@
       <c r="G81">
         <v>7</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="2">
         <v>11277</v>
       </c>
       <c r="I81">
@@ -4340,7 +4401,7 @@
       <c r="G82">
         <v>300</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="2">
         <v>328200</v>
       </c>
       <c r="I82">
@@ -4387,7 +4448,7 @@
       <c r="G83">
         <v>300</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="2">
         <v>1138050</v>
       </c>
       <c r="I83">
@@ -4434,7 +4495,7 @@
       <c r="G84">
         <v>125</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="2">
         <v>70875</v>
       </c>
       <c r="I84">
@@ -4481,7 +4542,7 @@
       <c r="G85">
         <v>350</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="2">
         <v>444150</v>
       </c>
       <c r="I85">
@@ -4528,7 +4589,7 @@
       <c r="G86">
         <v>350</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="2">
         <v>444150</v>
       </c>
       <c r="I86">
@@ -4575,7 +4636,7 @@
       <c r="G87">
         <v>7</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="2">
         <v>5733</v>
       </c>
       <c r="I87">
@@ -4622,7 +4683,7 @@
       <c r="G88">
         <v>15</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="2">
         <v>24457.5</v>
       </c>
       <c r="I88">
@@ -4669,7 +4730,7 @@
       <c r="G89">
         <v>125</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="2">
         <v>239500</v>
       </c>
       <c r="I89">
@@ -4716,7 +4777,7 @@
       <c r="G90">
         <v>125</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="2">
         <v>316125</v>
       </c>
       <c r="I90">
@@ -4763,7 +4824,7 @@
       <c r="G91">
         <v>350</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="2">
         <v>784000</v>
       </c>
       <c r="I91">
@@ -4810,7 +4871,7 @@
       <c r="G92">
         <v>12</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="2">
         <v>42246</v>
       </c>
       <c r="I92">
@@ -4857,7 +4918,7 @@
       <c r="G93">
         <v>350</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="2">
         <v>247450</v>
       </c>
       <c r="I93">
@@ -4904,7 +4965,7 @@
       <c r="G94">
         <v>15</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="2">
         <v>5760</v>
       </c>
       <c r="I94">
@@ -4951,7 +5012,7 @@
       <c r="G95">
         <v>12</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="2">
         <v>23244</v>
       </c>
       <c r="I95">
@@ -4998,7 +5059,7 @@
       <c r="G96">
         <v>15</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="2">
         <v>23400</v>
       </c>
       <c r="I96">
@@ -5045,7 +5106,7 @@
       <c r="G97">
         <v>300</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="2">
         <v>261900</v>
       </c>
       <c r="I97">
@@ -5092,7 +5153,7 @@
       <c r="G98">
         <v>350</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="2">
         <v>736575</v>
       </c>
       <c r="I98">
@@ -5139,7 +5200,7 @@
       <c r="G99">
         <v>12</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="2">
         <v>48312</v>
       </c>
       <c r="I99">
@@ -5186,7 +5247,7 @@
       <c r="G100">
         <v>20</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="2">
         <v>47880</v>
       </c>
       <c r="I100">
@@ -5233,7 +5294,7 @@
       <c r="G101">
         <v>300</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="2">
         <v>409800</v>
       </c>
       <c r="I101">
@@ -5280,7 +5341,7 @@
       <c r="G102">
         <v>7</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="2">
         <v>12656</v>
       </c>
       <c r="I102">
@@ -5327,7 +5388,7 @@
       <c r="G103">
         <v>20</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="2">
         <v>58700</v>
       </c>
       <c r="I103">
@@ -5374,7 +5435,7 @@
       <c r="G104">
         <v>125</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="2">
         <v>302000</v>
       </c>
       <c r="I104">
@@ -5421,7 +5482,7 @@
       <c r="G105">
         <v>15</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="2">
         <v>40335</v>
       </c>
       <c r="I105">
@@ -5468,7 +5529,7 @@
       <c r="G106">
         <v>7</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="2">
         <v>19138</v>
       </c>
       <c r="I106">
@@ -5515,7 +5576,7 @@
       <c r="G107">
         <v>12</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="2">
         <v>25308</v>
       </c>
       <c r="I107">
@@ -5562,7 +5623,7 @@
       <c r="G108">
         <v>350</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="2">
         <v>218050</v>
       </c>
       <c r="I108">
@@ -5609,7 +5670,7 @@
       <c r="G109">
         <v>7</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="2">
         <v>19138</v>
       </c>
       <c r="I109">
@@ -5656,7 +5717,7 @@
       <c r="G110">
         <v>12</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="2">
         <v>33132</v>
       </c>
       <c r="I110">
@@ -5703,7 +5764,7 @@
       <c r="G111">
         <v>350</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="2">
         <v>323050</v>
       </c>
       <c r="I111">
@@ -5750,7 +5811,7 @@
       <c r="G112">
         <v>20</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="2">
         <v>24980</v>
       </c>
       <c r="I112">
@@ -5797,7 +5858,7 @@
       <c r="G113">
         <v>350</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="2">
         <v>921200</v>
       </c>
       <c r="I113">
@@ -5844,7 +5905,7 @@
       <c r="G114">
         <v>125</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="2">
         <v>197875</v>
       </c>
       <c r="I114">
@@ -5891,7 +5952,7 @@
       <c r="G115">
         <v>15</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="2">
         <v>23475</v>
       </c>
       <c r="I115">
@@ -5938,7 +5999,7 @@
       <c r="G116">
         <v>20</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="2">
         <v>24980</v>
       </c>
       <c r="I116">
@@ -5985,7 +6046,7 @@
       <c r="G117">
         <v>350</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="2">
         <v>921200</v>
       </c>
       <c r="I117">
@@ -6032,7 +6093,7 @@
       <c r="G118">
         <v>125</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="2">
         <v>197875</v>
       </c>
       <c r="I118">
@@ -6079,7 +6140,7 @@
       <c r="G119">
         <v>15</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="2">
         <v>23475</v>
       </c>
       <c r="I119">
@@ -6126,7 +6187,7 @@
       <c r="G120">
         <v>125</v>
       </c>
-      <c r="H120">
+      <c r="H120" s="2">
         <v>207375</v>
       </c>
       <c r="I120">
@@ -6173,7 +6234,7 @@
       <c r="G121">
         <v>20</v>
       </c>
-      <c r="H121">
+      <c r="H121" s="2">
         <v>48560</v>
       </c>
       <c r="I121">
@@ -6220,7 +6281,7 @@
       <c r="G122">
         <v>300</v>
       </c>
-      <c r="H122">
+      <c r="H122" s="2">
         <v>448800</v>
       </c>
       <c r="I122">
@@ -6267,7 +6328,7 @@
       <c r="G123">
         <v>15</v>
       </c>
-      <c r="H123">
+      <c r="H123" s="2">
         <v>34500</v>
       </c>
       <c r="I123">
@@ -6314,7 +6375,7 @@
       <c r="G124">
         <v>350</v>
       </c>
-      <c r="H124">
+      <c r="H124" s="2">
         <v>779625</v>
       </c>
       <c r="I124">
@@ -6361,7 +6422,7 @@
       <c r="G125">
         <v>350</v>
       </c>
-      <c r="H125">
+      <c r="H125" s="2">
         <v>70000</v>
       </c>
       <c r="I125">
@@ -6408,7 +6469,7 @@
       <c r="G126">
         <v>7</v>
       </c>
-      <c r="H126">
+      <c r="H126" s="2">
         <v>2716</v>
       </c>
       <c r="I126">
@@ -6455,7 +6516,7 @@
       <c r="G127">
         <v>15</v>
       </c>
-      <c r="H127">
+      <c r="H127" s="2">
         <v>34500</v>
       </c>
       <c r="I127">
@@ -6502,7 +6563,7 @@
       <c r="G128">
         <v>15</v>
       </c>
-      <c r="H128">
+      <c r="H128" s="2">
         <v>37050</v>
       </c>
       <c r="I128">
@@ -6549,7 +6610,7 @@
       <c r="G129">
         <v>15</v>
       </c>
-      <c r="H129">
+      <c r="H129" s="2">
         <v>26145</v>
       </c>
       <c r="I129">
@@ -6596,7 +6657,7 @@
       <c r="G130">
         <v>350</v>
       </c>
-      <c r="H130">
+      <c r="H130" s="2">
         <v>245000</v>
       </c>
       <c r="I130">
@@ -6643,7 +6704,7 @@
       <c r="G131">
         <v>12</v>
       </c>
-      <c r="H131">
+      <c r="H131" s="2">
         <v>26664</v>
       </c>
       <c r="I131">
@@ -6690,7 +6751,7 @@
       <c r="G132">
         <v>300</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="2">
         <v>80700</v>
       </c>
       <c r="I132">
@@ -6737,7 +6798,7 @@
       <c r="G133">
         <v>300</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="2">
         <v>80700</v>
       </c>
       <c r="I133">
@@ -6784,7 +6845,7 @@
       <c r="G134">
         <v>300</v>
       </c>
-      <c r="H134">
+      <c r="H134" s="2">
         <v>448800</v>
       </c>
       <c r="I134">
@@ -6831,7 +6892,7 @@
       <c r="G135">
         <v>300</v>
       </c>
-      <c r="H135">
+      <c r="H135" s="2">
         <v>266400</v>
       </c>
       <c r="I135">
@@ -6878,7 +6939,7 @@
       <c r="G136">
         <v>15</v>
       </c>
-      <c r="H136">
+      <c r="H136" s="2">
         <v>26145</v>
       </c>
       <c r="I136">
@@ -6925,7 +6986,7 @@
       <c r="G137">
         <v>15</v>
       </c>
-      <c r="H137">
+      <c r="H137" s="2">
         <v>24210</v>
       </c>
       <c r="I137">
@@ -6972,7 +7033,7 @@
       <c r="G138">
         <v>15</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="2">
         <v>38385</v>
       </c>
       <c r="I138">
@@ -7019,7 +7080,7 @@
       <c r="G139">
         <v>20</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="2">
         <v>17310</v>
       </c>
       <c r="I139">
@@ -7066,7 +7127,7 @@
       <c r="G140">
         <v>125</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="2">
         <v>369250</v>
       </c>
       <c r="I140">
@@ -7113,7 +7174,7 @@
       <c r="G141">
         <v>7</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="2">
         <v>5061</v>
       </c>
       <c r="I141">

</xml_diff>